<commit_message>
Travailler sur manuel technique
</commit_message>
<xml_diff>
--- a/Materiel/ListeDePieces.xlsx
+++ b/Materiel/ListeDePieces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cegep\Hiver2024\Projet\ProjetFinalTSO_Serrebrooke\Materiel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3677855-5535-4FA2-977E-AC5BFD65F793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B702154-CB1C-4442-959F-1565F5295EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C79740FE-A834-484F-933F-D24615D948F3}"/>
   </bookViews>
@@ -122,9 +122,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -162,7 +162,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -268,7 +268,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -410,7 +410,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -421,7 +421,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,7 +466,7 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>